<commit_message>
added 1st version of table
</commit_message>
<xml_diff>
--- a/TestData/dataset_properties.xlsx
+++ b/TestData/dataset_properties.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elliot\Desktop\TU Graz courses\Semester 4 (SS 2021)\vizopt-fx\Datasets\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elliot\Desktop\TU Graz courses\Semester 4 (SS 2021)\pcp-tool\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600F233E-70CB-430A-AA4D-D97400F8046D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{079D5AD8-AACF-41AA-A077-3994B0A7689D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Dataset</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>2C_6_mod</t>
+  </si>
+  <si>
+    <t>Number of dim orderings (factorial)</t>
   </si>
 </sst>
 </file>
@@ -403,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,9 +418,10 @@
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="33.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -430,8 +434,11 @@
       <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -444,8 +451,12 @@
       <c r="D2" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="1">
+        <f>FACT(D2)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -458,8 +469,12 @@
       <c r="D3" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="1">
+        <f t="shared" ref="E3:E9" si="0">FACT(D3)</f>
+        <v>5040</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -472,8 +487,12 @@
       <c r="D4" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="1">
+        <f t="shared" si="0"/>
+        <v>720</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -486,8 +505,12 @@
       <c r="D5" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="1">
+        <f t="shared" si="0"/>
+        <v>40320</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -500,8 +523,12 @@
       <c r="D6" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="1">
+        <f t="shared" si="0"/>
+        <v>5040</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -514,8 +541,12 @@
       <c r="D7" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="1">
+        <f t="shared" si="0"/>
+        <v>5040</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -528,8 +559,12 @@
       <c r="D8" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -541,6 +576,10 @@
       </c>
       <c r="D9" s="2">
         <v>5</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="0"/>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>